<commit_message>
fixing bugs in main
</commit_message>
<xml_diff>
--- a/data/Experimental_Project_days_template.xlsx
+++ b/data/Experimental_Project_days_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ExcelWizard\ExcelWizard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ECBF850-2EA7-4274-8A7F-DD9D87C9C86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1533479B-4BA8-46E0-90C4-DD27F0452925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="604" xr2:uid="{782AB68F-678C-48D2-BD57-CBB026018020}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="604" activeTab="1" xr2:uid="{782AB68F-678C-48D2-BD57-CBB026018020}"/>
   </bookViews>
   <sheets>
     <sheet name="WD" sheetId="3" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="95">
   <si>
     <t>Role Ending</t>
   </si>
@@ -1392,11 +1392,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8460C7E-38BD-4E5B-AB0A-57D3C75D7B69}">
   <dimension ref="A1:BE103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10919,32 +10919,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8D3E9A9-514E-4262-B93A-789A2723EA54}">
-  <dimension ref="A1:AS38"/>
+  <dimension ref="A1:AR38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="3" max="3" width="31.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9.25" customWidth="1"/>
-    <col min="10" max="10" width="20.4140625" customWidth="1"/>
-    <col min="36" max="43" width="8.75" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="8" max="8" width="9.25" customWidth="1"/>
+    <col min="9" max="9" width="20.4140625" customWidth="1"/>
+    <col min="35" max="42" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="43" x14ac:dyDescent="0.4">
-      <c r="B1" s="1"/>
-      <c r="C1" s="33"/>
+    <row r="1" spans="1:44" ht="43" x14ac:dyDescent="0.4">
+      <c r="B1" s="33"/>
+      <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
@@ -10960,8 +10962,8 @@
       <c r="O1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>8</v>
+      <c r="P1" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>9</v>
@@ -10987,8 +10989,8 @@
       <c r="X1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="Y1" s="3" t="s">
-        <v>9</v>
+      <c r="Y1" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>10</v>
@@ -10999,8 +11001,8 @@
       <c r="AB1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AC1" s="4" t="s">
-        <v>10</v>
+      <c r="AC1" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="AD1" s="5" t="s">
         <v>11</v>
@@ -11017,14 +11019,14 @@
       <c r="AH1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AI1" s="5" t="s">
-        <v>11</v>
+      <c r="AI1" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="AJ1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AK1" s="6" t="s">
-        <v>12</v>
+      <c r="AK1" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="AL1" s="7" t="s">
         <v>13</v>
@@ -11041,250 +11043,245 @@
       <c r="AP1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AQ1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="9"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="9"/>
     </row>
-    <row r="2" spans="1:45" ht="70" x14ac:dyDescent="0.3">
-      <c r="A2" s="36">
-        <v>45292</v>
-      </c>
-      <c r="B2" s="1"/>
+    <row r="2" spans="1:44" ht="70" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="42" t="s">
         <v>60</v>
       </c>
+      <c r="F2" s="19" t="s">
+        <v>2</v>
+      </c>
       <c r="G2" s="19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="19" t="s">
         <v>58</v>
       </c>
+      <c r="J2" s="29" t="s">
+        <v>14</v>
+      </c>
       <c r="K2" s="29" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="29" t="s">
         <v>19</v>
       </c>
+      <c r="P2" s="11" t="s">
+        <v>20</v>
+      </c>
       <c r="Q2" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="S2" s="11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y2" s="11" t="s">
         <v>28</v>
       </c>
+      <c r="Y2" s="30" t="s">
+        <v>29</v>
+      </c>
       <c r="Z2" s="30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AA2" s="30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AB2" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC2" s="30" t="s">
         <v>32</v>
       </c>
+      <c r="AC2" s="17" t="s">
+        <v>33</v>
+      </c>
       <c r="AD2" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AE2" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG2" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="AI2" s="17" t="s">
         <v>38</v>
       </c>
+      <c r="AI2" s="31" t="s">
+        <v>39</v>
+      </c>
       <c r="AJ2" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK2" s="31" t="s">
         <v>40</v>
       </c>
+      <c r="AK2" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="AL2" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AM2" s="32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AN2" s="32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AO2" s="32" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AP2" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="AR2" s="11" t="s">
+      <c r="AQ2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AS2" s="10" t="s">
+      <c r="AR2" s="10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="36">
         <v>45292</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C3" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="38">
+      <c r="D3" s="38">
         <v>24</v>
       </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="37" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="39">
-        <f>E3</f>
+      <c r="G3" s="39">
+        <f>D3</f>
         <v>24</v>
       </c>
-      <c r="I3" s="40">
-        <f t="shared" ref="I3:I4" si="0">H3-SUM(K3:AS3)</f>
+      <c r="H3" s="40">
+        <f t="shared" ref="H3:H4" si="0">G3-SUM(J3:AR3)</f>
         <v>4</v>
       </c>
-      <c r="J3" s="41"/>
-      <c r="K3" s="1">
+      <c r="I3" s="41"/>
+      <c r="J3" s="1">
         <v>1</v>
       </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1">
+      <c r="P3" s="1">
         <v>2</v>
       </c>
+      <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1">
+      <c r="T3" s="1">
         <v>3</v>
       </c>
+      <c r="U3" s="1"/>
       <c r="V3" s="1"/>
       <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="26"/>
+      <c r="X3" s="26"/>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1">
+      <c r="AB3" s="1">
         <v>13</v>
       </c>
+      <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
-      <c r="AJ3" s="26">
+      <c r="AI3" s="26">
         <v>1</v>
       </c>
+      <c r="AJ3" s="1"/>
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
+      <c r="AQ3" s="46"/>
       <c r="AR3" s="46"/>
-      <c r="AS3" s="46"/>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="36">
         <v>45292</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C4" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="38">
+      <c r="D4" s="38">
         <v>14</v>
       </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="37" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="39">
-        <f>E4</f>
+      <c r="G4" s="39">
+        <f>D4</f>
         <v>14</v>
       </c>
-      <c r="I4" s="40">
+      <c r="H4" s="40">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
+      <c r="I4" s="41"/>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -11293,14 +11290,14 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1">
+      <c r="T4" s="1">
         <v>1</v>
       </c>
+      <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="26"/>
+      <c r="X4" s="26"/>
+      <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
@@ -11315,16 +11312,15 @@
       <c r="AK4" s="1"/>
       <c r="AL4" s="1"/>
       <c r="AM4" s="1"/>
-      <c r="AN4" s="1"/>
-      <c r="AO4" s="26">
+      <c r="AN4" s="26">
         <v>1</v>
       </c>
+      <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
-      <c r="AQ4" s="1"/>
+      <c r="AQ4" s="46"/>
       <c r="AR4" s="46"/>
-      <c r="AS4" s="46"/>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="77">
         <v>45292</v>
       </c>
@@ -11335,19 +11331,22 @@
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="G5" s="14">
+        <f>SUM(G3:G4)</f>
+        <v>38</v>
+      </c>
       <c r="H5" s="14">
         <f>SUM(H3:H4)</f>
-        <v>38</v>
-      </c>
-      <c r="I5" s="14">
-        <f>SUM(I3:I4)</f>
         <v>16</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14">
+        <f t="shared" ref="J5:AR5" si="1">SUM(J3:J4)</f>
+        <v>1</v>
+      </c>
       <c r="K5" s="14">
-        <f t="shared" ref="K5:AS5" si="1">SUM(K3:K4)</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="L5" s="14">
         <f t="shared" si="1"/>
@@ -11367,11 +11366,11 @@
       </c>
       <c r="P5" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R5" s="14">
         <f t="shared" si="1"/>
@@ -11383,11 +11382,11 @@
       </c>
       <c r="T5" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U5" s="14">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V5" s="14">
         <f t="shared" si="1"/>
@@ -11415,11 +11414,11 @@
       </c>
       <c r="AB5" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="AC5" s="14">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="AD5" s="14">
         <f t="shared" si="1"/>
@@ -11443,11 +11442,11 @@
       </c>
       <c r="AI5" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="14">
         <f t="shared" si="1"/>
@@ -11463,11 +11462,11 @@
       </c>
       <c r="AN5" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP5" s="14">
         <f t="shared" si="1"/>
@@ -11481,55 +11480,51 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AS5" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="36">
         <v>45323</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C6" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="38">
+      <c r="D6" s="38">
         <v>24</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="37" t="s">
+      <c r="E6" s="38"/>
+      <c r="F6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="39">
-        <f>E6</f>
+      <c r="G6" s="39">
+        <f>D6</f>
         <v>24</v>
       </c>
-      <c r="I6" s="40">
-        <f t="shared" ref="I6:I7" si="2">H6-SUM(K6:AS6)</f>
+      <c r="H6" s="40">
+        <f t="shared" ref="H6:H7" si="2">G6-SUM(J6:AR6)</f>
         <v>23</v>
       </c>
-      <c r="J6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="26"/>
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26">
+      <c r="M6" s="26">
         <v>1</v>
       </c>
+      <c r="N6" s="26"/>
       <c r="O6" s="26"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="26"/>
       <c r="R6" s="26"/>
       <c r="S6" s="26"/>
       <c r="T6" s="26"/>
-      <c r="U6" s="26"/>
+      <c r="U6" s="44"/>
       <c r="V6" s="44"/>
       <c r="W6" s="44"/>
       <c r="X6" s="44"/>
-      <c r="Y6" s="44"/>
+      <c r="Y6" s="26"/>
       <c r="Z6" s="26"/>
       <c r="AA6" s="26"/>
       <c r="AB6" s="26"/>
@@ -11547,54 +11542,53 @@
       <c r="AN6" s="26"/>
       <c r="AO6" s="26"/>
       <c r="AP6" s="26"/>
-      <c r="AQ6" s="26"/>
+      <c r="AQ6" s="47"/>
       <c r="AR6" s="47"/>
-      <c r="AS6" s="47"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="36">
         <v>45323</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C7" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="38">
+      <c r="D7" s="38">
         <v>14</v>
       </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="37" t="s">
+      <c r="E7" s="38"/>
+      <c r="F7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="39">
-        <f>E7</f>
+      <c r="G7" s="39">
+        <f>D7</f>
         <v>14</v>
       </c>
-      <c r="I7" s="40">
+      <c r="H7" s="40">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="J7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26">
-        <v>0</v>
-      </c>
+      <c r="M7" s="26">
+        <v>0</v>
+      </c>
+      <c r="N7" s="26"/>
       <c r="O7" s="26"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
       <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
+      <c r="U7" s="44"/>
       <c r="V7" s="44"/>
       <c r="W7" s="44"/>
       <c r="X7" s="44"/>
-      <c r="Y7" s="44"/>
+      <c r="Y7" s="26"/>
       <c r="Z7" s="26"/>
       <c r="AA7" s="26"/>
       <c r="AB7" s="26"/>
@@ -11612,11 +11606,10 @@
       <c r="AN7" s="26"/>
       <c r="AO7" s="26"/>
       <c r="AP7" s="26"/>
-      <c r="AQ7" s="26"/>
+      <c r="AQ7" s="47"/>
       <c r="AR7" s="47"/>
-      <c r="AS7" s="47"/>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="77">
         <v>45323</v>
       </c>
@@ -11627,18 +11620,21 @@
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="14">
+        <f>SUM(G6:G7)</f>
+        <v>38</v>
+      </c>
       <c r="H8" s="14">
         <f>SUM(H6:H7)</f>
-        <v>38</v>
-      </c>
-      <c r="I8" s="14">
-        <f>SUM(I6:I7)</f>
         <v>37</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14">
+        <f t="shared" ref="J8:AR8" si="3">SUM(J6:J7)</f>
+        <v>0</v>
+      </c>
       <c r="K8" s="14">
-        <f t="shared" ref="K8:AS8" si="3">SUM(K6:K7)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L8" s="14">
@@ -11647,11 +11643,11 @@
       </c>
       <c r="M8" s="14">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="14">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="14">
         <f t="shared" si="3"/>
@@ -11773,128 +11769,123 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AS8" s="14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" s="36">
         <v>45352</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C9" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="38">
+      <c r="D9" s="38">
         <v>24</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="37" t="s">
+      <c r="E9" s="38"/>
+      <c r="F9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="39">
-        <f>E9</f>
+      <c r="G9" s="39">
+        <f>D9</f>
         <v>24</v>
       </c>
-      <c r="I9" s="40">
-        <f t="shared" ref="I9:I10" si="4">H9-SUM(L9:AS9)</f>
+      <c r="H9" s="40">
+        <f t="shared" ref="H9:H10" si="4">G9-SUM(K9:AR9)</f>
         <v>3</v>
       </c>
-      <c r="J9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="26">
+      <c r="M9" s="26">
         <v>1</v>
       </c>
+      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1">
+      <c r="Q9" s="1">
         <v>2</v>
       </c>
+      <c r="R9" s="26"/>
       <c r="S9" s="26"/>
-      <c r="T9" s="26"/>
-      <c r="U9" s="26">
+      <c r="T9" s="26">
         <v>2</v>
       </c>
+      <c r="U9" s="44"/>
       <c r="V9" s="44"/>
       <c r="W9" s="44"/>
       <c r="X9" s="44"/>
-      <c r="Y9" s="44"/>
+      <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1">
+      <c r="AB9" s="1">
         <v>15</v>
       </c>
+      <c r="AC9" s="1"/>
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="49"/>
-      <c r="AJ9" s="26">
+      <c r="AH9" s="49"/>
+      <c r="AI9" s="26">
         <v>1</v>
       </c>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="56"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="56"/>
+      <c r="AL9" s="1"/>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
       <c r="AP9" s="1"/>
-      <c r="AQ9" s="1"/>
+      <c r="AQ9" s="46"/>
       <c r="AR9" s="46"/>
-      <c r="AS9" s="46"/>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" s="36">
         <v>45352</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C10" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="38">
+      <c r="D10" s="38">
         <v>14</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="37" t="s">
+      <c r="E10" s="38"/>
+      <c r="F10" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="39">
-        <f>E10</f>
+      <c r="G10" s="39">
+        <f>D10</f>
         <v>14</v>
       </c>
-      <c r="I10" s="40">
+      <c r="H10" s="40">
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="J10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+      <c r="R10" s="26"/>
       <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26">
+      <c r="T10" s="26">
         <v>1</v>
       </c>
+      <c r="U10" s="44"/>
       <c r="V10" s="44"/>
       <c r="W10" s="44"/>
       <c r="X10" s="44"/>
-      <c r="Y10" s="44"/>
+      <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
@@ -11904,21 +11895,20 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
+      <c r="AI10" s="60"/>
       <c r="AJ10" s="60"/>
-      <c r="AK10" s="60"/>
+      <c r="AK10" s="1"/>
       <c r="AL10" s="1"/>
       <c r="AM10" s="1"/>
-      <c r="AN10" s="1"/>
-      <c r="AO10" s="26">
+      <c r="AN10" s="26">
         <v>1</v>
       </c>
+      <c r="AO10" s="1"/>
       <c r="AP10" s="1"/>
-      <c r="AQ10" s="1"/>
+      <c r="AQ10" s="46"/>
       <c r="AR10" s="46"/>
-      <c r="AS10" s="46"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" s="77">
         <v>45353</v>
       </c>
@@ -11929,18 +11919,21 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="14">
+        <f>SUM(G9:G10)</f>
+        <v>38</v>
+      </c>
       <c r="H11" s="14">
         <f>SUM(H9:H10)</f>
-        <v>38</v>
-      </c>
-      <c r="I11" s="14">
-        <f>SUM(I9:I10)</f>
         <v>15</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14">
+        <f t="shared" ref="J11:AR11" si="5">SUM(J9:J10)</f>
+        <v>0</v>
+      </c>
       <c r="K11" s="14">
-        <f t="shared" ref="K11:AS11" si="5">SUM(K9:K10)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L11" s="14">
@@ -11949,11 +11942,11 @@
       </c>
       <c r="M11" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="14">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="14">
         <f t="shared" si="5"/>
@@ -11965,11 +11958,11 @@
       </c>
       <c r="Q11" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R11" s="14">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S11" s="14">
         <f t="shared" si="5"/>
@@ -11977,11 +11970,11 @@
       </c>
       <c r="T11" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U11" s="14">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="V11" s="14">
         <f t="shared" si="5"/>
@@ -12009,11 +12002,11 @@
       </c>
       <c r="AB11" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AC11" s="14">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="AD11" s="14">
         <f t="shared" si="5"/>
@@ -12037,11 +12030,11 @@
       </c>
       <c r="AI11" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11" s="14">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK11" s="14">
         <f t="shared" si="5"/>
@@ -12057,11 +12050,11 @@
       </c>
       <c r="AN11" s="14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO11" s="14">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP11" s="14">
         <f t="shared" si="5"/>
@@ -12075,53 +12068,49 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AS11" s="14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" s="36">
         <v>45383</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C12" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="38">
+      <c r="D12" s="38">
         <v>24</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="37" t="s">
+      <c r="E12" s="38"/>
+      <c r="F12" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="39">
-        <f>E12</f>
+      <c r="G12" s="39">
+        <f>D12</f>
         <v>24</v>
       </c>
-      <c r="I12" s="40">
-        <f t="shared" ref="I12:I13" si="6">H12-SUM(K12:AS12)</f>
+      <c r="H12" s="40">
+        <f t="shared" ref="H12:H13" si="6">G12-SUM(J12:AR12)</f>
         <v>24</v>
       </c>
-      <c r="J12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="1"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="26"/>
       <c r="S12" s="26"/>
       <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
+      <c r="U12" s="44"/>
       <c r="V12" s="44"/>
       <c r="W12" s="44"/>
       <c r="X12" s="44"/>
-      <c r="Y12" s="44"/>
+      <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
@@ -12131,60 +12120,59 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="26"/>
+      <c r="AI12" s="26"/>
+      <c r="AJ12" s="1"/>
       <c r="AK12" s="1"/>
       <c r="AL12" s="1"/>
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
       <c r="AP12" s="1"/>
-      <c r="AQ12" s="1"/>
+      <c r="AQ12" s="46"/>
       <c r="AR12" s="46"/>
-      <c r="AS12" s="46"/>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" s="36">
         <v>45383</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C13" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="38">
+      <c r="D13" s="38">
         <v>14</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="37" t="s">
+      <c r="E13" s="38"/>
+      <c r="F13" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="39">
-        <f>E13</f>
+      <c r="G13" s="39">
+        <f>D13</f>
         <v>14</v>
       </c>
-      <c r="I13" s="40">
+      <c r="H13" s="40">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="J13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="1"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="26"/>
       <c r="S13" s="26"/>
       <c r="T13" s="26"/>
-      <c r="U13" s="26"/>
+      <c r="U13" s="44"/>
       <c r="V13" s="44"/>
       <c r="W13" s="44"/>
       <c r="X13" s="44"/>
-      <c r="Y13" s="44"/>
+      <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
@@ -12199,14 +12187,13 @@
       <c r="AK13" s="1"/>
       <c r="AL13" s="1"/>
       <c r="AM13" s="1"/>
-      <c r="AN13" s="1"/>
-      <c r="AO13" s="26"/>
+      <c r="AN13" s="26"/>
+      <c r="AO13" s="1"/>
       <c r="AP13" s="1"/>
-      <c r="AQ13" s="1"/>
+      <c r="AQ13" s="46"/>
       <c r="AR13" s="46"/>
-      <c r="AS13" s="46"/>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" s="77">
         <v>45383</v>
       </c>
@@ -12217,18 +12204,21 @@
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="14">
+        <f>SUM(G12:G13)</f>
+        <v>38</v>
+      </c>
       <c r="H14" s="14">
         <f>SUM(H12:H13)</f>
         <v>38</v>
       </c>
-      <c r="I14" s="14">
-        <f>SUM(I12:I13)</f>
-        <v>38</v>
-      </c>
-      <c r="J14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14">
+        <f t="shared" ref="J14:AR14" si="7">SUM(J12:J13)</f>
+        <v>0</v>
+      </c>
       <c r="K14" s="14">
-        <f t="shared" ref="K14:AS14" si="7">SUM(K12:K13)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L14" s="14">
@@ -12363,53 +12353,49 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AS14" s="14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" s="36">
         <v>45413</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C15" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="38">
+      <c r="D15" s="38">
         <v>24</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="37" t="s">
+      <c r="E15" s="38"/>
+      <c r="F15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H15" s="39">
-        <f>E15</f>
+      <c r="G15" s="39">
+        <f>D15</f>
         <v>24</v>
       </c>
-      <c r="I15" s="40">
-        <f t="shared" ref="I15:I16" si="8">H15-SUM(K15:AS15)</f>
+      <c r="H15" s="40">
+        <f t="shared" ref="H15:H16" si="8">G15-SUM(J15:AR15)</f>
         <v>24</v>
       </c>
-      <c r="J15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="1"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="26"/>
       <c r="S15" s="26"/>
       <c r="T15" s="26"/>
-      <c r="U15" s="26"/>
+      <c r="U15" s="44"/>
       <c r="V15" s="44"/>
       <c r="W15" s="44"/>
       <c r="X15" s="44"/>
-      <c r="Y15" s="44"/>
+      <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
@@ -12419,60 +12405,59 @@
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
-      <c r="AJ15" s="26"/>
+      <c r="AI15" s="26"/>
+      <c r="AJ15" s="1"/>
       <c r="AK15" s="1"/>
       <c r="AL15" s="1"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
       <c r="AP15" s="1"/>
-      <c r="AQ15" s="1"/>
+      <c r="AQ15" s="46"/>
       <c r="AR15" s="46"/>
-      <c r="AS15" s="46"/>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" s="36">
         <v>45413</v>
       </c>
-      <c r="B16" s="1"/>
+      <c r="B16" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C16" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="38">
+      <c r="D16" s="38">
         <v>14</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="37" t="s">
+      <c r="E16" s="38"/>
+      <c r="F16" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="39">
-        <f>E16</f>
+      <c r="G16" s="39">
+        <f>D16</f>
         <v>14</v>
       </c>
-      <c r="I16" s="40">
+      <c r="H16" s="40">
         <f t="shared" si="8"/>
         <v>14</v>
       </c>
-      <c r="J16" s="41"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="1"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="26"/>
       <c r="S16" s="26"/>
       <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
+      <c r="U16" s="44"/>
       <c r="V16" s="44"/>
       <c r="W16" s="44"/>
       <c r="X16" s="44"/>
-      <c r="Y16" s="44"/>
+      <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
@@ -12487,14 +12472,13 @@
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
-      <c r="AN16" s="1"/>
-      <c r="AO16" s="26"/>
+      <c r="AN16" s="26"/>
+      <c r="AO16" s="1"/>
       <c r="AP16" s="1"/>
-      <c r="AQ16" s="1"/>
+      <c r="AQ16" s="46"/>
       <c r="AR16" s="46"/>
-      <c r="AS16" s="46"/>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A17" s="77">
         <v>45413</v>
       </c>
@@ -12505,18 +12489,21 @@
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="14">
+        <f>SUM(G15:G16)</f>
+        <v>38</v>
+      </c>
       <c r="H17" s="14">
         <f>SUM(H15:H16)</f>
         <v>38</v>
       </c>
-      <c r="I17" s="14">
-        <f>SUM(I15:I16)</f>
-        <v>38</v>
-      </c>
-      <c r="J17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14">
+        <f t="shared" ref="J17:AR17" si="9">SUM(J15:J16)</f>
+        <v>0</v>
+      </c>
       <c r="K17" s="14">
-        <f t="shared" ref="K17:AS17" si="9">SUM(K15:K16)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="L17" s="14">
@@ -12651,53 +12638,49 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AS17" s="14">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A18" s="36">
         <v>45444</v>
       </c>
-      <c r="B18" s="1"/>
+      <c r="B18" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C18" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D18" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="38">
+      <c r="D18" s="38">
         <v>24</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="37" t="s">
+      <c r="E18" s="38"/>
+      <c r="F18" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="39">
-        <f>E18</f>
+      <c r="G18" s="39">
+        <f>D18</f>
         <v>24</v>
       </c>
-      <c r="I18" s="40">
-        <f t="shared" ref="I18:I19" si="10">H18-SUM(K18:AS18)</f>
+      <c r="H18" s="40">
+        <f t="shared" ref="H18:H19" si="10">G18-SUM(J18:AR18)</f>
         <v>24</v>
       </c>
-      <c r="J18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="1"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="26"/>
       <c r="S18" s="26"/>
       <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
+      <c r="U18" s="44"/>
       <c r="V18" s="44"/>
       <c r="W18" s="44"/>
       <c r="X18" s="44"/>
-      <c r="Y18" s="44"/>
+      <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
@@ -12707,60 +12690,59 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
-      <c r="AI18" s="1"/>
-      <c r="AJ18" s="26"/>
+      <c r="AI18" s="26"/>
+      <c r="AJ18" s="1"/>
       <c r="AK18" s="1"/>
       <c r="AL18" s="1"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
       <c r="AP18" s="1"/>
-      <c r="AQ18" s="1"/>
+      <c r="AQ18" s="46"/>
       <c r="AR18" s="46"/>
-      <c r="AS18" s="46"/>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A19" s="36">
         <v>45444</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C19" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="38">
+      <c r="D19" s="38">
         <v>14</v>
       </c>
-      <c r="F19" s="38"/>
-      <c r="G19" s="37" t="s">
+      <c r="E19" s="38"/>
+      <c r="F19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H19" s="39">
-        <f>E19</f>
+      <c r="G19" s="39">
+        <f>D19</f>
         <v>14</v>
       </c>
-      <c r="I19" s="40">
+      <c r="H19" s="40">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="J19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="1"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="26"/>
       <c r="S19" s="26"/>
       <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
+      <c r="U19" s="44"/>
       <c r="V19" s="44"/>
       <c r="W19" s="44"/>
       <c r="X19" s="44"/>
-      <c r="Y19" s="44"/>
+      <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
@@ -12775,14 +12757,13 @@
       <c r="AK19" s="1"/>
       <c r="AL19" s="1"/>
       <c r="AM19" s="1"/>
-      <c r="AN19" s="1"/>
-      <c r="AO19" s="26"/>
+      <c r="AN19" s="26"/>
+      <c r="AO19" s="1"/>
       <c r="AP19" s="1"/>
-      <c r="AQ19" s="1"/>
+      <c r="AQ19" s="46"/>
       <c r="AR19" s="46"/>
-      <c r="AS19" s="46"/>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A20" s="77">
         <v>45444</v>
       </c>
@@ -12793,18 +12774,21 @@
       <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="G20" s="14">
+        <f>SUM(G18:G19)</f>
+        <v>38</v>
+      </c>
       <c r="H20" s="14">
         <f>SUM(H18:H19)</f>
         <v>38</v>
       </c>
-      <c r="I20" s="14">
-        <f>SUM(I18:I19)</f>
-        <v>38</v>
-      </c>
-      <c r="J20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14">
+        <f t="shared" ref="J20:AR20" si="11">SUM(J18:J19)</f>
+        <v>0</v>
+      </c>
       <c r="K20" s="14">
-        <f t="shared" ref="K20:AS20" si="11">SUM(K18:K19)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="L20" s="14">
@@ -12939,53 +12923,49 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AS20" s="14">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A21" s="36">
         <v>45474</v>
       </c>
-      <c r="B21" s="1"/>
+      <c r="B21" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C21" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="38">
+      <c r="D21" s="38">
         <v>24</v>
       </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="37" t="s">
+      <c r="E21" s="38"/>
+      <c r="F21" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="39">
-        <f>E21</f>
+      <c r="G21" s="39">
+        <f>D21</f>
         <v>24</v>
       </c>
-      <c r="I21" s="40">
-        <f t="shared" ref="I21:I22" si="12">H21-SUM(K21:AS21)</f>
+      <c r="H21" s="40">
+        <f t="shared" ref="H21:H22" si="12">G21-SUM(J21:AR21)</f>
         <v>24</v>
       </c>
-      <c r="J21" s="41"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="1"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="26"/>
       <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="44"/>
       <c r="V21" s="44"/>
       <c r="W21" s="44"/>
       <c r="X21" s="44"/>
-      <c r="Y21" s="44"/>
+      <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
@@ -12995,60 +12975,59 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
-      <c r="AI21" s="1"/>
-      <c r="AJ21" s="26"/>
+      <c r="AI21" s="26"/>
+      <c r="AJ21" s="1"/>
       <c r="AK21" s="1"/>
       <c r="AL21" s="1"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
       <c r="AP21" s="1"/>
-      <c r="AQ21" s="1"/>
+      <c r="AQ21" s="46"/>
       <c r="AR21" s="46"/>
-      <c r="AS21" s="46"/>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A22" s="36">
         <v>45474</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C22" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="38">
+      <c r="D22" s="38">
         <v>14</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="37" t="s">
+      <c r="E22" s="38"/>
+      <c r="F22" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="39">
-        <f>E22</f>
+      <c r="G22" s="39">
+        <f>D22</f>
         <v>14</v>
       </c>
-      <c r="I22" s="40">
+      <c r="H22" s="40">
         <f t="shared" si="12"/>
         <v>14</v>
       </c>
-      <c r="J22" s="41"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="1"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="26"/>
       <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="44"/>
       <c r="V22" s="44"/>
       <c r="W22" s="44"/>
       <c r="X22" s="44"/>
-      <c r="Y22" s="44"/>
+      <c r="Y22" s="1"/>
       <c r="Z22" s="1"/>
       <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
@@ -13063,14 +13042,13 @@
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
       <c r="AM22" s="1"/>
-      <c r="AN22" s="1"/>
-      <c r="AO22" s="26"/>
+      <c r="AN22" s="26"/>
+      <c r="AO22" s="1"/>
       <c r="AP22" s="1"/>
-      <c r="AQ22" s="1"/>
+      <c r="AQ22" s="46"/>
       <c r="AR22" s="46"/>
-      <c r="AS22" s="46"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A23" s="77">
         <v>45474</v>
       </c>
@@ -13081,18 +13059,21 @@
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="G23" s="14">
+        <f>SUM(G21:G22)</f>
+        <v>38</v>
+      </c>
       <c r="H23" s="14">
         <f>SUM(H21:H22)</f>
         <v>38</v>
       </c>
-      <c r="I23" s="14">
-        <f>SUM(I21:I22)</f>
-        <v>38</v>
-      </c>
-      <c r="J23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14">
+        <f t="shared" ref="J23:AR23" si="13">SUM(J21:J22)</f>
+        <v>0</v>
+      </c>
       <c r="K23" s="14">
-        <f t="shared" ref="K23:AS23" si="13">SUM(K21:K22)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="L23" s="14">
@@ -13227,53 +13208,49 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AS23" s="14">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A24" s="36">
         <v>45505</v>
       </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C24" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="38">
+      <c r="D24" s="38">
         <v>24</v>
       </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="37" t="s">
+      <c r="E24" s="38"/>
+      <c r="F24" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="39">
-        <f>E24</f>
+      <c r="G24" s="39">
+        <f>D24</f>
         <v>24</v>
       </c>
-      <c r="I24" s="40">
-        <f t="shared" ref="I24:I25" si="14">H24-SUM(K24:AS24)</f>
+      <c r="H24" s="40">
+        <f t="shared" ref="H24:H25" si="14">G24-SUM(J24:AR24)</f>
         <v>24</v>
       </c>
-      <c r="J24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="1"/>
+      <c r="P24" s="26"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="26"/>
       <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="44"/>
       <c r="V24" s="44"/>
       <c r="W24" s="44"/>
       <c r="X24" s="44"/>
-      <c r="Y24" s="44"/>
+      <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -13283,60 +13260,59 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
-      <c r="AI24" s="1"/>
-      <c r="AJ24" s="26"/>
+      <c r="AI24" s="26"/>
+      <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
       <c r="AP24" s="1"/>
-      <c r="AQ24" s="1"/>
+      <c r="AQ24" s="46"/>
       <c r="AR24" s="46"/>
-      <c r="AS24" s="46"/>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A25" s="36">
         <v>45505</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C25" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="38">
+      <c r="D25" s="38">
         <v>14</v>
       </c>
-      <c r="F25" s="38"/>
-      <c r="G25" s="37" t="s">
+      <c r="E25" s="38"/>
+      <c r="F25" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H25" s="39">
-        <f>E25</f>
+      <c r="G25" s="39">
+        <f>D25</f>
         <v>14</v>
       </c>
-      <c r="I25" s="40">
+      <c r="H25" s="40">
         <f t="shared" si="14"/>
         <v>14</v>
       </c>
-      <c r="J25" s="41"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="1"/>
+      <c r="P25" s="26"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="26"/>
       <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="44"/>
       <c r="V25" s="44"/>
       <c r="W25" s="44"/>
       <c r="X25" s="44"/>
-      <c r="Y25" s="44"/>
+      <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
@@ -13351,14 +13327,13 @@
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
       <c r="AM25" s="1"/>
-      <c r="AN25" s="1"/>
-      <c r="AO25" s="26"/>
+      <c r="AN25" s="26"/>
+      <c r="AO25" s="1"/>
       <c r="AP25" s="1"/>
-      <c r="AQ25" s="1"/>
+      <c r="AQ25" s="46"/>
       <c r="AR25" s="46"/>
-      <c r="AS25" s="46"/>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A26" s="77">
         <v>45505</v>
       </c>
@@ -13369,18 +13344,21 @@
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="G26" s="14">
+        <f>SUM(G24:G25)</f>
+        <v>38</v>
+      </c>
       <c r="H26" s="14">
         <f>SUM(H24:H25)</f>
         <v>38</v>
       </c>
-      <c r="I26" s="14">
-        <f>SUM(I24:I25)</f>
-        <v>38</v>
-      </c>
-      <c r="J26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14">
+        <f t="shared" ref="J26:AR26" si="15">SUM(J24:J25)</f>
+        <v>0</v>
+      </c>
       <c r="K26" s="14">
-        <f t="shared" ref="K26:AS26" si="15">SUM(K24:K25)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="L26" s="14">
@@ -13515,53 +13493,49 @@
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="AS26" s="14">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A27" s="36">
         <v>45536</v>
       </c>
-      <c r="B27" s="1"/>
+      <c r="B27" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C27" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="38">
+      <c r="D27" s="38">
         <v>24</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="37" t="s">
+      <c r="E27" s="38"/>
+      <c r="F27" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="39">
-        <f>E27</f>
+      <c r="G27" s="39">
+        <f>D27</f>
         <v>24</v>
       </c>
-      <c r="I27" s="40">
-        <f t="shared" ref="I27:I28" si="16">H27-SUM(K27:AS27)</f>
+      <c r="H27" s="40">
+        <f t="shared" ref="H27:H28" si="16">G27-SUM(J27:AR27)</f>
         <v>24</v>
       </c>
-      <c r="J27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="1"/>
+      <c r="P27" s="26"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="26"/>
       <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="44"/>
       <c r="V27" s="44"/>
       <c r="W27" s="44"/>
       <c r="X27" s="44"/>
-      <c r="Y27" s="44"/>
+      <c r="Y27" s="1"/>
       <c r="Z27" s="1"/>
       <c r="AA27" s="1"/>
       <c r="AB27" s="1"/>
@@ -13571,60 +13545,59 @@
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
-      <c r="AI27" s="1"/>
-      <c r="AJ27" s="26"/>
+      <c r="AI27" s="26"/>
+      <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
       <c r="AL27" s="1"/>
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
       <c r="AP27" s="1"/>
-      <c r="AQ27" s="1"/>
+      <c r="AQ27" s="46"/>
       <c r="AR27" s="46"/>
-      <c r="AS27" s="46"/>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A28" s="36">
         <v>45536</v>
       </c>
-      <c r="B28" s="1"/>
+      <c r="B28" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C28" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="38">
+      <c r="D28" s="38">
         <v>14</v>
       </c>
-      <c r="F28" s="38"/>
-      <c r="G28" s="37" t="s">
+      <c r="E28" s="38"/>
+      <c r="F28" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="39">
-        <f>E28</f>
+      <c r="G28" s="39">
+        <f>D28</f>
         <v>14</v>
       </c>
-      <c r="I28" s="40">
+      <c r="H28" s="40">
         <f t="shared" si="16"/>
         <v>14</v>
       </c>
-      <c r="J28" s="41"/>
+      <c r="I28" s="41"/>
+      <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="1"/>
+      <c r="P28" s="26"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="26"/>
       <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="44"/>
       <c r="V28" s="44"/>
       <c r="W28" s="44"/>
       <c r="X28" s="44"/>
-      <c r="Y28" s="44"/>
+      <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
       <c r="AB28" s="1"/>
@@ -13639,14 +13612,13 @@
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
       <c r="AM28" s="1"/>
-      <c r="AN28" s="1"/>
-      <c r="AO28" s="26"/>
+      <c r="AN28" s="26"/>
+      <c r="AO28" s="1"/>
       <c r="AP28" s="1"/>
-      <c r="AQ28" s="1"/>
+      <c r="AQ28" s="46"/>
       <c r="AR28" s="46"/>
-      <c r="AS28" s="46"/>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A29" s="77">
         <v>45536</v>
       </c>
@@ -13657,18 +13629,21 @@
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="G29" s="14">
+        <f>SUM(G27:G28)</f>
+        <v>38</v>
+      </c>
       <c r="H29" s="14">
         <f>SUM(H27:H28)</f>
         <v>38</v>
       </c>
-      <c r="I29" s="14">
-        <f>SUM(I27:I28)</f>
-        <v>38</v>
-      </c>
-      <c r="J29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14">
+        <f t="shared" ref="J29:AR29" si="17">SUM(J27:J28)</f>
+        <v>0</v>
+      </c>
       <c r="K29" s="14">
-        <f t="shared" ref="K29:AS29" si="17">SUM(K27:K28)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="L29" s="14">
@@ -13803,53 +13778,49 @@
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="AS29" s="14">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
         <v>45566</v>
       </c>
-      <c r="B30" s="1"/>
+      <c r="B30" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C30" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E30" s="38">
+      <c r="D30" s="38">
         <v>24</v>
       </c>
-      <c r="F30" s="38"/>
-      <c r="G30" s="37" t="s">
+      <c r="E30" s="38"/>
+      <c r="F30" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H30" s="39">
-        <f>E30</f>
+      <c r="G30" s="39">
+        <f>D30</f>
         <v>24</v>
       </c>
-      <c r="I30" s="40">
-        <f t="shared" ref="I30:I31" si="18">H30-SUM(K30:AS30)</f>
+      <c r="H30" s="40">
+        <f t="shared" ref="H30:H31" si="18">G30-SUM(J30:AR30)</f>
         <v>24</v>
       </c>
-      <c r="J30" s="41"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="1"/>
+      <c r="P30" s="26"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="26"/>
       <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="44"/>
       <c r="V30" s="44"/>
       <c r="W30" s="44"/>
       <c r="X30" s="44"/>
-      <c r="Y30" s="44"/>
+      <c r="Y30" s="1"/>
       <c r="Z30" s="1"/>
       <c r="AA30" s="1"/>
       <c r="AB30" s="1"/>
@@ -13859,60 +13830,59 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
-      <c r="AI30" s="1"/>
-      <c r="AJ30" s="26"/>
+      <c r="AI30" s="26"/>
+      <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
       <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
       <c r="AP30" s="1"/>
-      <c r="AQ30" s="1"/>
+      <c r="AQ30" s="46"/>
       <c r="AR30" s="46"/>
-      <c r="AS30" s="46"/>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A31" s="36">
         <v>45566</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C31" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="38">
+      <c r="D31" s="38">
         <v>14</v>
       </c>
-      <c r="F31" s="38"/>
-      <c r="G31" s="37" t="s">
+      <c r="E31" s="38"/>
+      <c r="F31" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H31" s="39">
-        <f>E31</f>
+      <c r="G31" s="39">
+        <f>D31</f>
         <v>14</v>
       </c>
-      <c r="I31" s="40">
+      <c r="H31" s="40">
         <f t="shared" si="18"/>
         <v>14</v>
       </c>
-      <c r="J31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="1"/>
+      <c r="P31" s="26"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="26"/>
       <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
-      <c r="U31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="44"/>
       <c r="V31" s="44"/>
       <c r="W31" s="44"/>
       <c r="X31" s="44"/>
-      <c r="Y31" s="44"/>
+      <c r="Y31" s="1"/>
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
       <c r="AB31" s="1"/>
@@ -13927,14 +13897,13 @@
       <c r="AK31" s="1"/>
       <c r="AL31" s="1"/>
       <c r="AM31" s="1"/>
-      <c r="AN31" s="1"/>
-      <c r="AO31" s="26"/>
+      <c r="AN31" s="26"/>
+      <c r="AO31" s="1"/>
       <c r="AP31" s="1"/>
-      <c r="AQ31" s="1"/>
+      <c r="AQ31" s="46"/>
       <c r="AR31" s="46"/>
-      <c r="AS31" s="46"/>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A32" s="77">
         <v>45566</v>
       </c>
@@ -13945,18 +13914,21 @@
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="G32" s="14">
+        <f>SUM(G30:G31)</f>
+        <v>38</v>
+      </c>
       <c r="H32" s="14">
         <f>SUM(H30:H31)</f>
         <v>38</v>
       </c>
-      <c r="I32" s="14">
-        <f>SUM(I30:I31)</f>
-        <v>38</v>
-      </c>
-      <c r="J32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14">
+        <f t="shared" ref="J32:AR32" si="19">SUM(J30:J31)</f>
+        <v>0</v>
+      </c>
       <c r="K32" s="14">
-        <f t="shared" ref="K32:AS32" si="19">SUM(K30:K31)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L32" s="14">
@@ -14091,53 +14063,49 @@
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="AS32" s="14">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" s="36">
         <v>45597</v>
       </c>
-      <c r="B33" s="1"/>
+      <c r="B33" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C33" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="38">
+      <c r="D33" s="38">
         <v>24</v>
       </c>
-      <c r="F33" s="38"/>
-      <c r="G33" s="37" t="s">
+      <c r="E33" s="38"/>
+      <c r="F33" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H33" s="39">
-        <f>E33</f>
+      <c r="G33" s="39">
+        <f>D33</f>
         <v>24</v>
       </c>
-      <c r="I33" s="40">
-        <f t="shared" ref="I33:I34" si="20">H33-SUM(K33:AS33)</f>
+      <c r="H33" s="40">
+        <f t="shared" ref="H33:H34" si="20">G33-SUM(J33:AR33)</f>
         <v>24</v>
       </c>
-      <c r="J33" s="41"/>
+      <c r="I33" s="41"/>
+      <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="1"/>
+      <c r="P33" s="26"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="26"/>
       <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="44"/>
       <c r="V33" s="44"/>
       <c r="W33" s="44"/>
       <c r="X33" s="44"/>
-      <c r="Y33" s="44"/>
+      <c r="Y33" s="1"/>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
       <c r="AB33" s="1"/>
@@ -14147,60 +14115,59 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
-      <c r="AI33" s="1"/>
-      <c r="AJ33" s="26"/>
+      <c r="AI33" s="26"/>
+      <c r="AJ33" s="1"/>
       <c r="AK33" s="1"/>
       <c r="AL33" s="1"/>
       <c r="AM33" s="1"/>
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
       <c r="AP33" s="1"/>
-      <c r="AQ33" s="1"/>
+      <c r="AQ33" s="46"/>
       <c r="AR33" s="46"/>
-      <c r="AS33" s="46"/>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
         <v>45597</v>
       </c>
-      <c r="B34" s="1"/>
+      <c r="B34" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C34" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D34" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="38">
+      <c r="D34" s="38">
         <v>14</v>
       </c>
-      <c r="F34" s="38"/>
-      <c r="G34" s="37" t="s">
+      <c r="E34" s="38"/>
+      <c r="F34" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H34" s="39">
-        <f>E34</f>
+      <c r="G34" s="39">
+        <f>D34</f>
         <v>14</v>
       </c>
-      <c r="I34" s="40">
+      <c r="H34" s="40">
         <f t="shared" si="20"/>
         <v>14</v>
       </c>
-      <c r="J34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="1"/>
+      <c r="P34" s="26"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="26"/>
       <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
-      <c r="U34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="44"/>
       <c r="V34" s="44"/>
       <c r="W34" s="44"/>
       <c r="X34" s="44"/>
-      <c r="Y34" s="44"/>
+      <c r="Y34" s="1"/>
       <c r="Z34" s="1"/>
       <c r="AA34" s="1"/>
       <c r="AB34" s="1"/>
@@ -14215,14 +14182,13 @@
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
       <c r="AM34" s="1"/>
-      <c r="AN34" s="1"/>
-      <c r="AO34" s="26"/>
+      <c r="AN34" s="26"/>
+      <c r="AO34" s="1"/>
       <c r="AP34" s="1"/>
-      <c r="AQ34" s="1"/>
+      <c r="AQ34" s="46"/>
       <c r="AR34" s="46"/>
-      <c r="AS34" s="46"/>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" s="77">
         <v>45597</v>
       </c>
@@ -14233,18 +14199,21 @@
       <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="G35" s="14">
+        <f>SUM(G33:G34)</f>
+        <v>38</v>
+      </c>
       <c r="H35" s="14">
         <f>SUM(H33:H34)</f>
         <v>38</v>
       </c>
-      <c r="I35" s="14">
-        <f>SUM(I33:I34)</f>
-        <v>38</v>
-      </c>
-      <c r="J35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14">
+        <f t="shared" ref="J35:AR35" si="21">SUM(J33:J34)</f>
+        <v>0</v>
+      </c>
       <c r="K35" s="14">
-        <f t="shared" ref="K35:AS35" si="21">SUM(K33:K34)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L35" s="14">
@@ -14379,38 +14348,34 @@
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="AS35" s="14">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" s="36">
         <v>45627</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="37" t="s">
+        <v>55</v>
+      </c>
       <c r="C36" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="38">
+      <c r="D36" s="38">
         <v>24</v>
       </c>
-      <c r="F36" s="38"/>
-      <c r="G36" s="37" t="s">
+      <c r="E36" s="38"/>
+      <c r="F36" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H36" s="39">
-        <f>E36</f>
+      <c r="G36" s="39">
+        <f>D36</f>
         <v>24</v>
       </c>
-      <c r="I36" s="40">
-        <f t="shared" ref="I36:I37" si="22">H36-SUM(K36:AS36)</f>
+      <c r="H36" s="40">
+        <f t="shared" ref="H36:H37" si="22">G36-SUM(J36:AR36)</f>
         <v>24</v>
       </c>
-      <c r="J36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -14435,45 +14400,44 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
-      <c r="AI36" s="1"/>
-      <c r="AJ36" s="26"/>
+      <c r="AI36" s="26"/>
+      <c r="AJ36" s="1"/>
       <c r="AK36" s="1"/>
       <c r="AL36" s="1"/>
       <c r="AM36" s="1"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
       <c r="AP36" s="1"/>
-      <c r="AQ36" s="1"/>
+      <c r="AQ36" s="46"/>
       <c r="AR36" s="46"/>
-      <c r="AS36" s="46"/>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" s="36">
         <v>45627</v>
       </c>
-      <c r="B37" s="1"/>
+      <c r="B37" s="37" t="s">
+        <v>56</v>
+      </c>
       <c r="C37" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="D37" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="38">
+      <c r="D37" s="38">
         <v>14</v>
       </c>
-      <c r="F37" s="38"/>
-      <c r="G37" s="37" t="s">
+      <c r="E37" s="38"/>
+      <c r="F37" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="39">
-        <f>E37</f>
+      <c r="G37" s="39">
+        <f>D37</f>
         <v>14</v>
       </c>
-      <c r="I37" s="40">
+      <c r="H37" s="40">
         <f t="shared" si="22"/>
         <v>14</v>
       </c>
-      <c r="J37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -14503,14 +14467,13 @@
       <c r="AK37" s="1"/>
       <c r="AL37" s="1"/>
       <c r="AM37" s="1"/>
-      <c r="AN37" s="1"/>
-      <c r="AO37" s="26"/>
+      <c r="AN37" s="26"/>
+      <c r="AO37" s="1"/>
       <c r="AP37" s="1"/>
-      <c r="AQ37" s="1"/>
+      <c r="AQ37" s="46"/>
       <c r="AR37" s="46"/>
-      <c r="AS37" s="46"/>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" s="77">
         <v>45627</v>
       </c>
@@ -14521,18 +14484,21 @@
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
+      <c r="G38" s="14">
+        <f>SUM(G36:G37)</f>
+        <v>38</v>
+      </c>
       <c r="H38" s="14">
         <f>SUM(H36:H37)</f>
         <v>38</v>
       </c>
-      <c r="I38" s="14">
-        <f>SUM(I36:I37)</f>
-        <v>38</v>
-      </c>
-      <c r="J38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14">
+        <f t="shared" ref="J38:AR38" si="23">SUM(J36:J37)</f>
+        <v>0</v>
+      </c>
       <c r="K38" s="14">
-        <f t="shared" ref="K38:AS38" si="23">SUM(K36:K37)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L38" s="14">
@@ -14667,13 +14633,9 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="AS38" s="14">
-        <f t="shared" si="23"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I3:I4 I6:I7 I9:I10 I12:I13 I15:I16 I18:I19 I21:I22 I24:I25 I27:I28 I30:I31 I33:I34 I36:I37">
+  <conditionalFormatting sqref="H3:H4 H6:H7 H9:H10 H12:H13 H15:H16 H18:H19 H21:H22 H24:H25 H27:H28 H30:H31 H33:H34 H36:H37">
     <cfRule type="cellIs" dxfId="1" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>